<commit_message>
Actualizacion tipos de datos BSCS
</commit_message>
<xml_diff>
--- a/Proyecto_Grupo3/Diseño/Interfaces.xlsx
+++ b/Proyecto_Grupo3/Diseño/Interfaces.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14115" windowHeight="4680"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14115" windowHeight="4680" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Metodos" sheetId="1" r:id="rId1"/>
+    <sheet name="Tipos de Datos" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>Interfaces</t>
   </si>
@@ -97,6 +97,51 @@
   </si>
   <si>
     <t>Estado,mensaje</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Largo</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>STRING</t>
+  </si>
+  <si>
+    <t>Estado del Sistema</t>
+  </si>
+  <si>
+    <t>ID_CLIENTE</t>
+  </si>
+  <si>
+    <t>Identificador unico del Cliente. Llave primaria de la tabla Clientes</t>
+  </si>
+  <si>
+    <t>IMSI</t>
+  </si>
+  <si>
+    <t>INTEGER</t>
+  </si>
+  <si>
+    <t>MSISDN</t>
+  </si>
+  <si>
+    <t>Imsi del abonado</t>
+  </si>
+  <si>
+    <t>IMSISDN del Abonado</t>
+  </si>
+  <si>
+    <t>PLAN_BSCS</t>
+  </si>
+  <si>
+    <t>Plan En BSCS</t>
   </si>
 </sst>
 </file>
@@ -437,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +544,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -578,12 +623,102 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="59.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Se agrega tipo de datos DESC a planilla
</commit_message>
<xml_diff>
--- a/Proyecto_Grupo3/Diseño/Interfaces.xlsx
+++ b/Proyecto_Grupo3/Diseño/Interfaces.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>Interfaces</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>Plan En BSCS</t>
+  </si>
+  <si>
+    <t>DESC</t>
+  </si>
+  <si>
+    <t>Descripcion De respuestas</t>
   </si>
 </sst>
 </file>
@@ -623,10 +629,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,6 +722,20 @@
       </c>
       <c r="D6" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sistema Integrado y Funcionando. Ver 2 (incluido las mejoras de Mauricio)
</commit_message>
<xml_diff>
--- a/Proyecto_Grupo3/Diseño/Interfaces.xlsx
+++ b/Proyecto_Grupo3/Diseño/Interfaces.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>Interfaces</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>IMSI</t>
-  </si>
-  <si>
-    <t>INTEGER</t>
   </si>
   <si>
     <t>MSISDN</t>
@@ -644,7 +641,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B13:B14"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,32 +696,32 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C5">
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
@@ -733,12 +730,12 @@
         <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
@@ -747,12 +744,12 @@
         <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
         <v>31</v>
@@ -761,12 +758,12 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
         <v>31</v>
@@ -775,7 +772,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>